<commit_message>
Creating featuresets with NLTK
</commit_message>
<xml_diff>
--- a/web_crawler/su_dividendais.xlsx
+++ b/web_crawler/su_dividendais.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="189">
   <si>
     <t>Nuoroda</t>
   </si>
@@ -374,13 +374,220 @@
   </si>
   <si>
     <t>„Maxima grupė“</t>
+  </si>
+  <si>
+    <t>https://www.delfi.lt/pilietis/naujienos/kausto-nerimas-vilniuje-tvarkomos-gatves-iki-kitos-liuties.d?id=78578571</t>
+  </si>
+  <si>
+    <t>https://www.delfi.lt/auto/laisva-pavara/tamsioji-tesla-puse-darbuotojai-pasakoja-apie-braidziojima-po-srutas-ir-incidentu-nuslepimus.d?id=78598249</t>
+  </si>
+  <si>
+    <t>https://www.delfi.lt/veidai/zmones/klaipedoje-zuvusios-manekenes-byloje-kyla-itampa-isikisti-teko-ir-generalinei-prokuraturai.d?id=78599469</t>
+  </si>
+  <si>
+    <t>https://www.delfi.lt/news/daily/world/po-pasipiktinimo-bangos-del-susitikimo-su-putinu-neiprastas-trumpo-pareiskimas.d?id=78599005</t>
+  </si>
+  <si>
+    <t>https://www.delfi.lt/news/daily/lithuania/turi-plana-b-valstieciams-kirkilas-ivardijo-kas-galetu-buti-bendras-partiju-kandidatas-i-prezidentus.d?id=78599921</t>
+  </si>
+  <si>
+    <t>https://www.delfi.lt/news/daily/lithuania/staigmena-naujausiuose-kandidatu-i-prezidentus-reitinguose-lyderiu-trejetuke-ivyko-pokyciai.d?id=78582555</t>
+  </si>
+  <si>
+    <t>https://www.delfi.lt/sportas/futbolas/sensacija-kipre-gynyboje-uzsidariusi-suduva-is-turnyro-eliminavo-apoel-kluba.d?id=78598465#cxrecs_s</t>
+  </si>
+  <si>
+    <t>https://www.15min.lt/naujiena/aktualu/nusikaltimaiirnelaimes/imones-savininkas-beveik-puse-milijono-euru-pervede-tiesiai-sukciams-i-saskaita-59-1002668</t>
+  </si>
+  <si>
+    <t>https://www.15min.lt/naujiena/aktualu/lietuva/pastarosios-liutys-pridare-simtatukstantines-zalos-56-1002664</t>
+  </si>
+  <si>
+    <t>https://www.15min.lt/naujiena/aktualu/lietuva/palanga-aklavieteje-del-pavojingu-nutruktgalviu-su-paspirtukais-tures-bausti-visus-56-1000994</t>
+  </si>
+  <si>
+    <t>https://www.15min.lt/verslas/naujiena/transportas/nuplauke-tukstanciai-siltu-darbo-vietu-viskas-del-skrydzio-i-londona-667-1001992</t>
+  </si>
+  <si>
+    <t>https://www.15min.lt/naujiena/aktualu/pasaulis/d-trumpas-sutinka-kad-rusija-kisosi-i-rinkimus-teigia-ne-taip-isreiskes-minti-57-1002626</t>
+  </si>
+  <si>
+    <t>https://www.15min.lt/naujiena/aktualu/komentarai/marius-laurinavicius-d-trumpas-helsinkyje-nieko-neisdave-ir-nepardave-nes-neturejo-ka-500-1002584</t>
+  </si>
+  <si>
+    <t>https://www.15min.lt/naujiena/aktualu/lietuva/prezidento-rinkimu-reitingu-trejetukas-be-s-skvernelio-56-1002622</t>
+  </si>
+  <si>
+    <t>https://www.15min.lt/pasaulis-kiseneje/naujiena/kelioniu-pulsas/6-naujos-unesco-saugomos-vietos-europoje-637-1002474</t>
+  </si>
+  <si>
+    <t>https://www.15min.lt/verslas/naujiena/kvadratinis-metras/nekilnojamasis-turtas/palangoje-planuojamo-marriott-viesbucio-dar-teks-palaukti-973-1002024</t>
+  </si>
+  <si>
+    <t>https://www.15min.lt/sportas/naujiena/futbolas/prancuzu-talentas-paverge-pasauli-laimeta-premija-paaukojo-kilniam-tikslui-24-1002524</t>
+  </si>
+  <si>
+    <t>https://www.15min.lt/24sek/naujiena/kablys/pasaulio-futbolo-cempiono-pokstas-meile-nba-zaidejui-880-1002218</t>
+  </si>
+  <si>
+    <t>https://www.lrytas.lt/pasaulis/rytai-vakarai/2018/07/18/news/izeistas-jav-prezidentas-priesams-gali-kirsti-is-pasalu-6993313/</t>
+  </si>
+  <si>
+    <t>https://www.lrytas.lt/lietuvosdiena/aktualijos/2018/07/18/news/turi-plana-b-valstieciams-g-kirkilas-ivardijo-kas-galetu-buti-bendras-partiju-kandidatas-i-prezidentus-6995062/</t>
+  </si>
+  <si>
+    <t>https://www.lrytas.lt/verslas/rinkos-pulsas/2018/07/18/news/ispeja-pirkejus-saldytose-darzovese-rastas-mirtinas-uzkratas-6993291/</t>
+  </si>
+  <si>
+    <t>https://www.lrytas.lt/lietuvosdiena/aktualijos/2018/07/18/news/piju-is-naisiu-vasaros-nustebino-vrk-isvada-r-karbauskis-atvaziuodavo-tik-is-smalsumo--6993284/</t>
+  </si>
+  <si>
+    <t>https://www.lrytas.lt/bendraukime/man-rupi/2018/07/17/news/viesnage-londone-atvere-akis-pamacius-vietines-istiko-kulturinis-sokas--6953605/</t>
+  </si>
+  <si>
+    <t>https://www.lrytas.lt/verslas/sekmes-istorijos/2018/07/18/news/kauno-sekme-be-cia-kuriamu-gaminiu-neissivercia-pasaulines-imones-6981729/</t>
+  </si>
+  <si>
+    <t>https://www.lrytas.lt/sportas/futbolas/2018/07/18/news/futbolo-fabrikai-kurie-uzstrigo-rusijoje-cempionatui-truko-tik-vieno-dalyko-6989735/</t>
+  </si>
+  <si>
+    <t>https://www.lrytas.lt/sportas/futbolas/2018/07/17/news/svarbiausias-sezono-musis-suduva-isvykoje-kaunasi-su-apoel-6990974/</t>
+  </si>
+  <si>
+    <t>https://www.lrytas.lt/verslas/rinkos-pulsas/2018/07/17/news/lietuva-ir-ukraina-planuoja-naujus-tiesioginius-skrydzius-traukiniu-marsrutus-6990802/</t>
+  </si>
+  <si>
+    <t>https://www.lrytas.lt/verslas/rinkos-pulsas/2018/07/17/news/apie-artejancia-griuti-kalba-vis-dazniau-nera-abejoniu-kad-susidursime-su-krize-6949993/</t>
+  </si>
+  <si>
+    <t>https://www.lrytas.lt/verslas/rinkos-pulsas/2018/07/18/news/vietiniu-kova-su-turistais-draudzia-asmenukiu-lazdas-aukstakulnius-ir-tatuiruotes-6983258/</t>
+  </si>
+  <si>
+    <t>https://www.lrytas.lt/lietuvosdiena/aktualijos/2018/07/18/news/kuriamas-naujas-visuomeninis-judejimas-lietuvos-liberalai-atgaivina-liberalias-vertybes-6988861/</t>
+  </si>
+  <si>
+    <t>https://www.vz.lt/finansai-apskaita/2018/07/17/vmi-paaiskina-seimo-priimtus-gyventoju-pajamu-mokescio-pakeitimus</t>
+  </si>
+  <si>
+    <t>https://www.vz.lt/nekilnojamasis-turtas-statyba/2018/07/17/nordea-padalini-senamiestyje-keicia-bendradarbystes-erdve-restoranas-ir-parduotuve</t>
+  </si>
+  <si>
+    <t>https://www.vz.lt/nekilnojamasis-turtas-statyba/2018/07/18/auksciausioje-vilniaus-vietoje-suplanavo-16-isskirtines-architekturos-namu-kvartala</t>
+  </si>
+  <si>
+    <t>https://www.vz.lt/bankai-draudimas/2018/07/18/swedbank-lietuvoje-5-isaugino-grynaji-pelna</t>
+  </si>
+  <si>
+    <t>https://www.vz.lt/nekilnojamasis-turtas-statyba/2018/07/18/workland-planuoja-tolesne-pletra-vilniuje-investuos-15-mln-eur</t>
+  </si>
+  <si>
+    <t>https://www.vz.lt/vadyba/is-tarnybos-i/2018/07/18/devbridge-group-vilniaus-padalinys-turi-nauja-vadova</t>
+  </si>
+  <si>
+    <t>https://www.vz.lt/finansai-apskaita/2018/07/18/bankai-atsisako-klientu-o-pakiles-spiecius-iesko-naujo-avilio</t>
+  </si>
+  <si>
+    <t>https://www.vz.lt/pramone/2018/07/18/inhus-svedijoje-igyvendina-ypatinga-projekta-pasiruosimas-truko-metus</t>
+  </si>
+  <si>
+    <t>http://www.diena.lt/naujienos/vilnius/miesto-pulsas/pripazinimas-forbes-kelioniu-skiltyje-pagyros-vilniaus-senamiesciui-872898</t>
+  </si>
+  <si>
+    <t>http://www.diena.lt/naujienos/vilnius/miesto-pulsas/liuciu-apgadintu-dviraciu-taku-vilniuje-remontas-uztruks-dvi-savaites-872889</t>
+  </si>
+  <si>
+    <t>http://www.diena.lt/naujienos/lietuva/salies-pulsas/vokietijos-poligonuose-testuojami-lietuvai-pagaminti-sarvuociai-boxer-872974</t>
+  </si>
+  <si>
+    <t>http://www.diena.lt/naujienos/lietuva/politika/netiketumas-prezidento-rinkimu-reitingu-trejetukas-be-s-skvernelio-872944</t>
+  </si>
+  <si>
+    <t>http://www.diena.lt/galerijos/vaizdai/prezidente-susitiko-su-misija-sibiras-dalyviais-872961</t>
+  </si>
+  <si>
+    <t>http://www.diena.lt/galerijos/vaizdai/lkl-spaudos-konferencija-872939</t>
+  </si>
+  <si>
+    <t>http://www.diena.lt/naujienos/vilnius/nusikaltimai-ir-nelaimes/i-sukciu-spastus-papuole-imone-neteko-475-tukst-euru-872979</t>
+  </si>
+  <si>
+    <t>http://www.diena.lt/naujienos/kaunas/menas-ir-pramogos/unikali-bliuzo-kelione-nuo-memfio-iki-cikagos-ir-atgal-872960</t>
+  </si>
+  <si>
+    <t>http://www.diena.lt/naujienos/vilnius/nusikaltimai-ir-nelaimes/dviraciu-vagis-ikliuvo-su-ikalciais-872958</t>
+  </si>
+  <si>
+    <t>http://www.diena.lt/naujienos/vilnius/nusikaltimai-ir-nelaimes/vilniaus-rajone-dega-gyvenamasis-namas-872909</t>
+  </si>
+  <si>
+    <t>https://www.lzinios.lt/lzinios/Svietimas/sarada-mokytoju-per-daug-bet-ju-truksta/269210</t>
+  </si>
+  <si>
+    <t>https://www.lzinios.lt/lzinios/Komentarai/zvirbliu-isskris-juodaja-gulbe-sugris/269204</t>
+  </si>
+  <si>
+    <t>https://www.lzinios.lt/lzinios/Ekonomika/gyventojams-rupi-es-lesu-panaudojimas/269208</t>
+  </si>
+  <si>
+    <t>https://www.lzinios.lt/lzinios/Gimtasis-krastas/gedimino-kalno-situacija-stabili/269153</t>
+  </si>
+  <si>
+    <t>https://www.lzinios.lt/lzinios/Gimtasis-krastas/liuties-zala-sostines-dviraciu-takams-bus-likviduota-per-dvi-savaites/269176</t>
+  </si>
+  <si>
+    <t>https://www.lzinios.lt/lzinios/Lietuva/del-pensiju-reformos-kyla-i-nauja-musi/269131</t>
+  </si>
+  <si>
+    <t>https://www.lzinios.lt/lzinios/Lietuva/ko-reikia-kad-lrt-taptu-neitiketina/269130</t>
+  </si>
+  <si>
+    <t>https://www.lzinios.lt/lzinios/Gimtasis-krastas/remigijui-simasiui-nemalonumai-del-siuksliu-tesiasi/269169</t>
+  </si>
+  <si>
+    <t>https://www.lzinios.lt/lzinios/Mokslas-ir-svietimas/-google-street-view-grizta-i-lietuvos-kelius/269217</t>
+  </si>
+  <si>
+    <t>https://www.lzinios.lt/lzinios/Gimtasis-krastas/jaunimas-nori-pirkti-po-trupineli-pilies/269027</t>
+  </si>
+  <si>
+    <t>https://www.alfa.lt/straipsnis/50304445/po-pertraukos-prabude-neymaro-vedami-brazilai-pasaulio-cempionato-ketvirtfinalyje</t>
+  </si>
+  <si>
+    <t>https://www.alfa.lt/straipsnis/50308678/paaiskejo-daugiau-detaliu-apie-subsidijas-pirmam-bustui-apsidziaugs-ne-visi</t>
+  </si>
+  <si>
+    <t>https://www.alfa.lt/straipsnis/50308717/prie-seimo-galimai-nelegali-ledo-skulptura</t>
+  </si>
+  <si>
+    <t>https://www.alfa.lt/straipsnis/50308501/nt-rinka-kaune-investuotojai-neskuba-griebti-skaniu-bet-brangiu-kasneliu</t>
+  </si>
+  <si>
+    <t>https://www.alfa.lt/straipsnis/50308675/istorine-pergale-cempionu-lygoje-suduvai-garantavo-rekordine-pinigine-premija-is-uefa</t>
+  </si>
+  <si>
+    <t>https://www.alfa.lt/straipsnis/50308654/d-trumpas-persigalvojo-rusija-galejo-kistis-i-2016-m-rinkimus</t>
+  </si>
+  <si>
+    <t>https://www.alfa.lt/straipsnis/50308393/antroku-tevai-sukilo-del-pakeistos-mokytojos-direktorius-saiposi</t>
+  </si>
+  <si>
+    <t>https://www.alfa.lt/straipsnis/50307895/prancuzu-pergales-selsmas-nuo-paryziaus-iki-kauno</t>
+  </si>
+  <si>
+    <t>https://www.alfa.lt/straipsnis/50307697/d-trumpas-sulauze-ne-viena-karalisko-protokolo-taisykle-internautai-tai-palaike-nepagarbos-saliai-ir-karalienei-gestu</t>
+  </si>
+  <si>
+    <t>https://www.alfa.lt/straipsnis/50307235/po-vienos-itempciausiu-dienu-nato-istorijoje-d-grybauskaites-ir-d-trumpo-pokalbis-akis-i-aki-ka-vienas-kitam-pasake-prezidentai</t>
+  </si>
+  <si>
+    <t>https://www.alfa.lt/straipsnis/50308738/vmi-primena-apie-pamirstus-sumoketi-mokescius-laisku-sulauks-54-tukst-gyventoju</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,6 +736,15 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="186"/>
@@ -832,7 +1048,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -875,12 +1091,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -914,6 +1132,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1221,16 +1440,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
@@ -2928,7 +3147,583 @@
         <v>43293</v>
       </c>
     </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>120</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>121</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>122</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>123</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>124</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>125</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>126</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>127</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>128</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>130</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>131</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>132</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>133</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>134</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>135</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>136</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>137</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>138</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>139</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>140</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>141</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>142</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>143</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>144</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>144</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>145</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>146</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>147</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>148</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>149</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>150</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>151</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>152</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>153</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>154</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>155</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>156</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>157</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>158</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>159</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>160</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>161</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>162</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>163</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>178</v>
+      </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>179</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>180</v>
+      </c>
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>181</v>
+      </c>
+      <c r="B134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>182</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>183</v>
+      </c>
+      <c r="B136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>184</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>185</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>186</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>187</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>188</v>
+      </c>
+      <c r="B141">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A122" r:id="rId1"/>
+    <hyperlink ref="A129" r:id="rId2"/>
+    <hyperlink ref="A128" r:id="rId3"/>
+    <hyperlink ref="A127" r:id="rId4"/>
+    <hyperlink ref="A124" r:id="rId5"/>
+    <hyperlink ref="A130" r:id="rId6"/>
+    <hyperlink ref="A126" r:id="rId7"/>
+    <hyperlink ref="A125" r:id="rId8"/>
+    <hyperlink ref="A123" r:id="rId9"/>
+    <hyperlink ref="A121" r:id="rId10"/>
+    <hyperlink ref="A120" r:id="rId11"/>
+    <hyperlink ref="A119" r:id="rId12"/>
+    <hyperlink ref="A118" r:id="rId13"/>
+    <hyperlink ref="A117" r:id="rId14"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>